<commit_message>
24 April 2019 Moved Pop Unique to front of output file and ID label to index
</commit_message>
<xml_diff>
--- a/data/datasources/providers.xlsx
+++ b/data/datasources/providers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\pythoncode\myprojects\work\datagathering\data\datasources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A92940C3-C8CA-483B-BBDF-6C1DBFD30204}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D4336E4-3109-4104-9925-443EE97031BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E25E46C0-E192-4F16-9140-D9F8D222B765}"/>
+    <workbookView xWindow="14895" yWindow="2385" windowWidth="12405" windowHeight="14160" xr2:uid="{E25E46C0-E192-4F16-9140-D9F8D222B765}"/>
   </bookViews>
   <sheets>
     <sheet name="Providers" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="321">
   <si>
     <t>Emirates Integrated Telecommunications Company PJS</t>
   </si>
@@ -961,6 +961,33 @@
   </si>
   <si>
     <t>MNO Country</t>
+  </si>
+  <si>
+    <t>A&amp;F Networks B.V.</t>
+  </si>
+  <si>
+    <t>Al wafai International For Communication and Infor</t>
+  </si>
+  <si>
+    <t>Cogent Communications</t>
+  </si>
+  <si>
+    <t>GBI HQ Cooperatief U.A.</t>
+  </si>
+  <si>
+    <t>Ibrahim SEN</t>
+  </si>
+  <si>
+    <t>KoycegizNet Telekom</t>
+  </si>
+  <si>
+    <t>oja.at GmbH</t>
+  </si>
+  <si>
+    <t>Turuncunet Bilisim Iletisim Elekt. San. Tic. Ltd.</t>
+  </si>
+  <si>
+    <t>Integrated Tlecom Co. Ltd</t>
   </si>
 </sst>
 </file>
@@ -1321,11 +1348,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393946DC-22D6-469D-89E7-C1D77668D6CD}">
-  <dimension ref="A1:F251"/>
+  <dimension ref="A1:F260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,6 +1609,9 @@
       <c r="C16" t="s">
         <v>288</v>
       </c>
+      <c r="E16" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1663,6 +1693,9 @@
       <c r="C22" t="s">
         <v>289</v>
       </c>
+      <c r="E22" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1708,6 +1741,9 @@
       <c r="C25" t="s">
         <v>290</v>
       </c>
+      <c r="E25" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1747,6 +1783,9 @@
       <c r="C28" t="s">
         <v>291</v>
       </c>
+      <c r="E28" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -2872,47 +2911,47 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>101</v>
+        <v>315</v>
       </c>
       <c r="B101" t="s">
         <v>100</v>
       </c>
       <c r="C101" t="s">
-        <v>102</v>
-      </c>
-      <c r="D101" t="s">
-        <v>217</v>
+        <v>315</v>
       </c>
       <c r="E101" t="s">
-        <v>201</v>
-      </c>
-      <c r="F101">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s">
         <v>100</v>
       </c>
       <c r="C102" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="D102" t="s">
+        <v>217</v>
       </c>
       <c r="E102" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="F102">
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B103" t="s">
         <v>100</v>
       </c>
       <c r="C103" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E103" t="s">
         <v>200</v>
@@ -2920,13 +2959,13 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>238</v>
+        <v>104</v>
       </c>
       <c r="B104" t="s">
         <v>100</v>
       </c>
       <c r="C104" t="s">
-        <v>238</v>
+        <v>104</v>
       </c>
       <c r="E104" t="s">
         <v>200</v>
@@ -2934,47 +2973,47 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>238</v>
       </c>
       <c r="B105" t="s">
         <v>100</v>
       </c>
       <c r="C105" t="s">
-        <v>106</v>
-      </c>
-      <c r="D105" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="E105" t="s">
-        <v>201</v>
-      </c>
-      <c r="F105">
-        <v>2</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C106" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="D106" t="s">
+        <v>215</v>
       </c>
       <c r="E106" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="F106">
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B107" t="s">
         <v>107</v>
       </c>
       <c r="C107" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E107" t="s">
         <v>200</v>
@@ -2982,7 +3021,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B108" t="s">
         <v>107</v>
@@ -2996,13 +3035,13 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B109" t="s">
         <v>107</v>
       </c>
       <c r="C109" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E109" t="s">
         <v>200</v>
@@ -3010,13 +3049,13 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>239</v>
+        <v>111</v>
       </c>
       <c r="B110" t="s">
         <v>107</v>
       </c>
       <c r="C110" t="s">
-        <v>239</v>
+        <v>111</v>
       </c>
       <c r="E110" t="s">
         <v>200</v>
@@ -3024,13 +3063,13 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>239</v>
       </c>
       <c r="B111" t="s">
         <v>107</v>
       </c>
       <c r="C111" t="s">
-        <v>112</v>
+        <v>239</v>
       </c>
       <c r="E111" t="s">
         <v>200</v>
@@ -3038,13 +3077,13 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>313</v>
       </c>
       <c r="B112" t="s">
         <v>107</v>
       </c>
       <c r="C112" t="s">
-        <v>113</v>
+        <v>239</v>
       </c>
       <c r="E112" t="s">
         <v>200</v>
@@ -3052,13 +3091,13 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B113" t="s">
         <v>107</v>
       </c>
       <c r="C113" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E113" t="s">
         <v>200</v>
@@ -3066,13 +3105,13 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>296</v>
+        <v>113</v>
       </c>
       <c r="B114" t="s">
         <v>107</v>
       </c>
       <c r="C114" t="s">
-        <v>296</v>
+        <v>113</v>
       </c>
       <c r="E114" t="s">
         <v>200</v>
@@ -3080,13 +3119,13 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>297</v>
+        <v>114</v>
       </c>
       <c r="B115" t="s">
         <v>107</v>
       </c>
       <c r="C115" t="s">
-        <v>297</v>
+        <v>114</v>
       </c>
       <c r="E115" t="s">
         <v>200</v>
@@ -3094,13 +3133,13 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>240</v>
+        <v>296</v>
       </c>
       <c r="B116" t="s">
         <v>107</v>
       </c>
       <c r="C116" t="s">
-        <v>240</v>
+        <v>296</v>
       </c>
       <c r="E116" t="s">
         <v>200</v>
@@ -3108,13 +3147,13 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>241</v>
+        <v>297</v>
       </c>
       <c r="B117" t="s">
         <v>107</v>
       </c>
       <c r="C117" t="s">
-        <v>241</v>
+        <v>297</v>
       </c>
       <c r="E117" t="s">
         <v>200</v>
@@ -3122,13 +3161,13 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>115</v>
+        <v>240</v>
       </c>
       <c r="B118" t="s">
         <v>107</v>
       </c>
       <c r="C118" t="s">
-        <v>115</v>
+        <v>240</v>
       </c>
       <c r="E118" t="s">
         <v>200</v>
@@ -3136,13 +3175,13 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>116</v>
+        <v>241</v>
       </c>
       <c r="B119" t="s">
         <v>107</v>
       </c>
       <c r="C119" t="s">
-        <v>116</v>
+        <v>241</v>
       </c>
       <c r="E119" t="s">
         <v>200</v>
@@ -3150,13 +3189,13 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B120" t="s">
         <v>107</v>
       </c>
       <c r="C120" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E120" t="s">
         <v>200</v>
@@ -3164,78 +3203,78 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B121" t="s">
         <v>107</v>
       </c>
       <c r="C121" t="s">
-        <v>218</v>
-      </c>
-      <c r="D121" t="s">
-        <v>213</v>
+        <v>116</v>
       </c>
       <c r="E121" t="s">
-        <v>201</v>
-      </c>
-      <c r="F121">
-        <v>2</v>
+        <v>200</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B122" t="s">
         <v>107</v>
       </c>
       <c r="C122" t="s">
-        <v>204</v>
-      </c>
-      <c r="D122" t="s">
-        <v>216</v>
+        <v>117</v>
       </c>
       <c r="E122" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B123" t="s">
         <v>107</v>
       </c>
       <c r="C123" t="s">
-        <v>119</v>
+        <v>218</v>
+      </c>
+      <c r="D123" t="s">
+        <v>213</v>
       </c>
       <c r="E123" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="F123">
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>298</v>
+        <v>118</v>
       </c>
       <c r="B124" t="s">
         <v>107</v>
       </c>
       <c r="C124" t="s">
-        <v>119</v>
+        <v>204</v>
+      </c>
+      <c r="D124" t="s">
+        <v>216</v>
       </c>
       <c r="E124" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B125" t="s">
         <v>107</v>
       </c>
       <c r="C125" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E125" t="s">
         <v>200</v>
@@ -3243,13 +3282,13 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>242</v>
+        <v>298</v>
       </c>
       <c r="B126" t="s">
         <v>107</v>
       </c>
       <c r="C126" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E126" t="s">
         <v>200</v>
@@ -3257,13 +3296,13 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>121</v>
+        <v>320</v>
       </c>
       <c r="B127" t="s">
         <v>107</v>
       </c>
       <c r="C127" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E127" t="s">
         <v>200</v>
@@ -3271,13 +3310,13 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B128" t="s">
         <v>107</v>
       </c>
       <c r="C128" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E128" t="s">
         <v>200</v>
@@ -3285,13 +3324,13 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B129" t="s">
         <v>107</v>
       </c>
       <c r="C129" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="E129" t="s">
         <v>200</v>
@@ -3299,13 +3338,13 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>244</v>
+        <v>121</v>
       </c>
       <c r="B130" t="s">
         <v>107</v>
       </c>
       <c r="C130" t="s">
-        <v>244</v>
+        <v>121</v>
       </c>
       <c r="E130" t="s">
         <v>200</v>
@@ -3313,13 +3352,13 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B131" t="s">
         <v>107</v>
       </c>
       <c r="C131" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E131" t="s">
         <v>200</v>
@@ -3327,13 +3366,13 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B132" t="s">
         <v>107</v>
       </c>
       <c r="C132" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E132" t="s">
         <v>200</v>
@@ -3341,13 +3380,13 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>125</v>
+        <v>244</v>
       </c>
       <c r="B133" t="s">
         <v>107</v>
       </c>
       <c r="C133" t="s">
-        <v>125</v>
+        <v>244</v>
       </c>
       <c r="E133" t="s">
         <v>200</v>
@@ -3355,13 +3394,13 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B134" t="s">
         <v>107</v>
       </c>
       <c r="C134" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E134" t="s">
         <v>200</v>
@@ -3369,13 +3408,13 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>127</v>
+        <v>245</v>
       </c>
       <c r="B135" t="s">
         <v>107</v>
       </c>
       <c r="C135" t="s">
-        <v>127</v>
+        <v>245</v>
       </c>
       <c r="E135" t="s">
         <v>200</v>
@@ -3383,13 +3422,13 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>246</v>
+        <v>125</v>
       </c>
       <c r="B136" t="s">
         <v>107</v>
       </c>
       <c r="C136" t="s">
-        <v>246</v>
+        <v>125</v>
       </c>
       <c r="E136" t="s">
         <v>200</v>
@@ -3397,13 +3436,13 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B137" t="s">
         <v>107</v>
       </c>
       <c r="C137" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E137" t="s">
         <v>200</v>
@@ -3411,13 +3450,13 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>129</v>
+        <v>318</v>
       </c>
       <c r="B138" t="s">
         <v>107</v>
       </c>
       <c r="C138" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="E138" t="s">
         <v>200</v>
@@ -3425,13 +3464,13 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>247</v>
+        <v>127</v>
       </c>
       <c r="B139" t="s">
         <v>107</v>
       </c>
       <c r="C139" t="s">
-        <v>247</v>
+        <v>127</v>
       </c>
       <c r="E139" t="s">
         <v>200</v>
@@ -3439,33 +3478,27 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>130</v>
+        <v>246</v>
       </c>
       <c r="B140" t="s">
         <v>107</v>
       </c>
       <c r="C140" t="s">
-        <v>131</v>
-      </c>
-      <c r="D140" t="s">
-        <v>211</v>
+        <v>246</v>
       </c>
       <c r="E140" t="s">
-        <v>201</v>
-      </c>
-      <c r="F140">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B141" t="s">
         <v>107</v>
       </c>
       <c r="C141" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E141" t="s">
         <v>200</v>
@@ -3473,13 +3506,13 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B142" t="s">
         <v>107</v>
       </c>
       <c r="C142" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E142" t="s">
         <v>200</v>
@@ -3487,257 +3520,263 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>134</v>
+        <v>247</v>
       </c>
       <c r="B143" t="s">
         <v>107</v>
       </c>
       <c r="C143" t="s">
-        <v>134</v>
-      </c>
-      <c r="D143" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="E143" t="s">
-        <v>201</v>
-      </c>
-      <c r="F143">
-        <v>3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>130</v>
+      </c>
+      <c r="B144" t="s">
+        <v>107</v>
+      </c>
+      <c r="C144" t="s">
+        <v>131</v>
+      </c>
+      <c r="D144" t="s">
+        <v>211</v>
+      </c>
+      <c r="E144" t="s">
+        <v>201</v>
+      </c>
+      <c r="F144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>132</v>
+      </c>
+      <c r="B145" t="s">
+        <v>107</v>
+      </c>
+      <c r="C145" t="s">
+        <v>132</v>
+      </c>
+      <c r="E145" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>133</v>
+      </c>
+      <c r="B146" t="s">
+        <v>107</v>
+      </c>
+      <c r="C146" t="s">
+        <v>133</v>
+      </c>
+      <c r="E146" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>134</v>
+      </c>
+      <c r="B147" t="s">
+        <v>107</v>
+      </c>
+      <c r="C147" t="s">
+        <v>134</v>
+      </c>
+      <c r="D147" t="s">
+        <v>212</v>
+      </c>
+      <c r="E147" t="s">
+        <v>201</v>
+      </c>
+      <c r="F147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>136</v>
       </c>
-      <c r="B144" t="s">
-        <v>135</v>
-      </c>
-      <c r="C144" t="s">
+      <c r="B148" t="s">
+        <v>135</v>
+      </c>
+      <c r="C148" t="s">
         <v>136</v>
       </c>
-      <c r="E144" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+      <c r="E148" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>312</v>
+      </c>
+      <c r="B149" t="s">
+        <v>135</v>
+      </c>
+      <c r="C149" t="s">
+        <v>312</v>
+      </c>
+      <c r="E149" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>248</v>
       </c>
-      <c r="B145" t="s">
-        <v>135</v>
-      </c>
-      <c r="C145" t="s">
+      <c r="B150" t="s">
+        <v>135</v>
+      </c>
+      <c r="C150" t="s">
         <v>249</v>
       </c>
-      <c r="E145" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+      <c r="E150" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>137</v>
       </c>
-      <c r="B146" t="s">
-        <v>135</v>
-      </c>
-      <c r="C146" t="s">
+      <c r="B151" t="s">
+        <v>135</v>
+      </c>
+      <c r="C151" t="s">
         <v>137</v>
       </c>
-      <c r="E146" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="E151" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>138</v>
       </c>
-      <c r="B147" t="s">
-        <v>135</v>
-      </c>
-      <c r="C147" t="s">
+      <c r="B152" t="s">
+        <v>135</v>
+      </c>
+      <c r="C152" t="s">
         <v>138</v>
       </c>
-      <c r="E147" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="E152" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>250</v>
       </c>
-      <c r="B148" t="s">
-        <v>135</v>
-      </c>
-      <c r="C148" t="s">
+      <c r="B153" t="s">
+        <v>135</v>
+      </c>
+      <c r="C153" t="s">
         <v>250</v>
       </c>
-      <c r="E148" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="E153" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>251</v>
       </c>
-      <c r="B149" t="s">
-        <v>135</v>
-      </c>
-      <c r="C149" t="s">
+      <c r="B154" t="s">
+        <v>135</v>
+      </c>
+      <c r="C154" t="s">
         <v>251</v>
       </c>
-      <c r="E149" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="E154" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>139</v>
       </c>
-      <c r="B150" t="s">
-        <v>135</v>
-      </c>
-      <c r="C150" t="s">
+      <c r="B155" t="s">
+        <v>135</v>
+      </c>
+      <c r="C155" t="s">
         <v>139</v>
       </c>
-      <c r="E150" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="E155" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>141</v>
       </c>
-      <c r="B151" t="s">
-        <v>135</v>
-      </c>
-      <c r="C151" t="s">
+      <c r="B156" t="s">
+        <v>135</v>
+      </c>
+      <c r="C156" t="s">
         <v>141</v>
       </c>
-      <c r="E151" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="E156" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>140</v>
       </c>
-      <c r="B152" t="s">
-        <v>135</v>
-      </c>
-      <c r="C152" t="s">
+      <c r="B157" t="s">
+        <v>135</v>
+      </c>
+      <c r="C157" t="s">
         <v>141</v>
       </c>
-      <c r="E152" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="E157" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>299</v>
       </c>
-      <c r="B153" t="s">
-        <v>135</v>
-      </c>
-      <c r="C153" t="s">
+      <c r="B158" t="s">
+        <v>135</v>
+      </c>
+      <c r="C158" t="s">
         <v>141</v>
       </c>
-      <c r="E153" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="E158" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>309</v>
       </c>
-      <c r="B154" t="s">
-        <v>135</v>
-      </c>
-      <c r="C154" t="s">
+      <c r="B159" t="s">
+        <v>135</v>
+      </c>
+      <c r="C159" t="s">
         <v>141</v>
       </c>
-      <c r="E154" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="E159" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>142</v>
       </c>
-      <c r="B155" t="s">
-        <v>135</v>
-      </c>
-      <c r="C155" t="s">
+      <c r="B160" t="s">
+        <v>135</v>
+      </c>
+      <c r="C160" t="s">
         <v>142</v>
-      </c>
-      <c r="E155" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>143</v>
-      </c>
-      <c r="B156" t="s">
-        <v>135</v>
-      </c>
-      <c r="C156" t="s">
-        <v>143</v>
-      </c>
-      <c r="E156" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>144</v>
-      </c>
-      <c r="B157" t="s">
-        <v>135</v>
-      </c>
-      <c r="C157" t="s">
-        <v>144</v>
-      </c>
-      <c r="E157" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>252</v>
-      </c>
-      <c r="B158" t="s">
-        <v>135</v>
-      </c>
-      <c r="C158" t="s">
-        <v>253</v>
-      </c>
-      <c r="E158" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>254</v>
-      </c>
-      <c r="B159" t="s">
-        <v>135</v>
-      </c>
-      <c r="C159" t="s">
-        <v>254</v>
-      </c>
-      <c r="E159" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>255</v>
-      </c>
-      <c r="B160" t="s">
-        <v>135</v>
-      </c>
-      <c r="C160" t="s">
-        <v>255</v>
       </c>
       <c r="E160" t="s">
         <v>200</v>
@@ -3745,13 +3784,13 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B161" t="s">
         <v>135</v>
       </c>
       <c r="C161" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E161" t="s">
         <v>200</v>
@@ -3759,13 +3798,13 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B162" t="s">
         <v>135</v>
       </c>
       <c r="C162" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E162" t="s">
         <v>200</v>
@@ -3773,13 +3812,13 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>147</v>
+        <v>252</v>
       </c>
       <c r="B163" t="s">
         <v>135</v>
       </c>
       <c r="C163" t="s">
-        <v>147</v>
+        <v>253</v>
       </c>
       <c r="E163" t="s">
         <v>200</v>
@@ -3787,13 +3826,13 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>148</v>
+        <v>254</v>
       </c>
       <c r="B164" t="s">
         <v>135</v>
       </c>
       <c r="C164" t="s">
-        <v>148</v>
+        <v>254</v>
       </c>
       <c r="E164" t="s">
         <v>200</v>
@@ -3801,13 +3840,13 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>149</v>
+        <v>255</v>
       </c>
       <c r="B165" t="s">
         <v>135</v>
       </c>
       <c r="C165" t="s">
-        <v>149</v>
+        <v>255</v>
       </c>
       <c r="E165" t="s">
         <v>200</v>
@@ -3815,13 +3854,13 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>256</v>
+        <v>145</v>
       </c>
       <c r="B166" t="s">
         <v>135</v>
       </c>
       <c r="C166" t="s">
-        <v>256</v>
+        <v>145</v>
       </c>
       <c r="E166" t="s">
         <v>200</v>
@@ -3829,13 +3868,13 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B167" t="s">
         <v>135</v>
       </c>
       <c r="C167" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E167" t="s">
         <v>200</v>
@@ -3843,13 +3882,13 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>300</v>
+        <v>147</v>
       </c>
       <c r="B168" t="s">
         <v>135</v>
       </c>
       <c r="C168" t="s">
-        <v>300</v>
+        <v>147</v>
       </c>
       <c r="E168" t="s">
         <v>200</v>
@@ -3857,13 +3896,13 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B169" t="s">
         <v>135</v>
       </c>
       <c r="C169" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E169" t="s">
         <v>200</v>
@@ -3871,13 +3910,13 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B170" t="s">
         <v>135</v>
       </c>
       <c r="C170" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E170" t="s">
         <v>200</v>
@@ -3885,13 +3924,13 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B171" t="s">
         <v>135</v>
       </c>
       <c r="C171" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E171" t="s">
         <v>200</v>
@@ -3899,13 +3938,13 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>258</v>
+        <v>150</v>
       </c>
       <c r="B172" t="s">
         <v>135</v>
       </c>
       <c r="C172" t="s">
-        <v>258</v>
+        <v>150</v>
       </c>
       <c r="E172" t="s">
         <v>200</v>
@@ -3913,13 +3952,13 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>153</v>
+        <v>300</v>
       </c>
       <c r="B173" t="s">
         <v>135</v>
       </c>
       <c r="C173" t="s">
-        <v>153</v>
+        <v>300</v>
       </c>
       <c r="E173" t="s">
         <v>200</v>
@@ -3927,13 +3966,13 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B174" t="s">
         <v>135</v>
       </c>
       <c r="C174" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E174" t="s">
         <v>200</v>
@@ -3941,13 +3980,13 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>259</v>
+        <v>152</v>
       </c>
       <c r="B175" t="s">
         <v>135</v>
       </c>
       <c r="C175" t="s">
-        <v>259</v>
+        <v>152</v>
       </c>
       <c r="E175" t="s">
         <v>200</v>
@@ -3955,13 +3994,13 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>301</v>
+        <v>257</v>
       </c>
       <c r="B176" t="s">
         <v>135</v>
       </c>
       <c r="C176" t="s">
-        <v>301</v>
+        <v>257</v>
       </c>
       <c r="E176" t="s">
         <v>200</v>
@@ -3969,13 +4008,13 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>302</v>
+        <v>258</v>
       </c>
       <c r="B177" t="s">
         <v>135</v>
       </c>
       <c r="C177" t="s">
-        <v>302</v>
+        <v>258</v>
       </c>
       <c r="E177" t="s">
         <v>200</v>
@@ -3983,13 +4022,13 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B178" t="s">
         <v>135</v>
       </c>
       <c r="C178" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E178" t="s">
         <v>200</v>
@@ -3997,13 +4036,13 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>260</v>
+        <v>154</v>
       </c>
       <c r="B179" t="s">
         <v>135</v>
       </c>
       <c r="C179" t="s">
-        <v>260</v>
+        <v>154</v>
       </c>
       <c r="E179" t="s">
         <v>200</v>
@@ -4011,13 +4050,13 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>156</v>
+        <v>259</v>
       </c>
       <c r="B180" t="s">
         <v>135</v>
       </c>
       <c r="C180" t="s">
-        <v>156</v>
+        <v>259</v>
       </c>
       <c r="E180" t="s">
         <v>200</v>
@@ -4025,13 +4064,13 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B181" t="s">
         <v>135</v>
       </c>
       <c r="C181" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E181" t="s">
         <v>200</v>
@@ -4039,13 +4078,13 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>261</v>
+        <v>302</v>
       </c>
       <c r="B182" t="s">
         <v>135</v>
       </c>
       <c r="C182" t="s">
-        <v>261</v>
+        <v>302</v>
       </c>
       <c r="E182" t="s">
         <v>200</v>
@@ -4053,13 +4092,13 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B183" t="s">
         <v>135</v>
       </c>
       <c r="C183" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E183" t="s">
         <v>200</v>
@@ -4067,13 +4106,13 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B184" t="s">
         <v>135</v>
       </c>
       <c r="C184" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E184" t="s">
         <v>200</v>
@@ -4081,13 +4120,13 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>263</v>
+        <v>156</v>
       </c>
       <c r="B185" t="s">
         <v>135</v>
       </c>
       <c r="C185" t="s">
-        <v>263</v>
+        <v>156</v>
       </c>
       <c r="E185" t="s">
         <v>200</v>
@@ -4095,13 +4134,13 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B186" t="s">
         <v>135</v>
       </c>
       <c r="C186" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E186" t="s">
         <v>200</v>
@@ -4109,13 +4148,13 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>158</v>
+        <v>316</v>
       </c>
       <c r="B187" t="s">
         <v>135</v>
       </c>
       <c r="C187" t="s">
-        <v>158</v>
+        <v>316</v>
       </c>
       <c r="E187" t="s">
         <v>200</v>
@@ -4123,13 +4162,13 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B188" t="s">
         <v>135</v>
       </c>
       <c r="C188" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E188" t="s">
         <v>200</v>
@@ -4137,13 +4176,13 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>265</v>
+        <v>157</v>
       </c>
       <c r="B189" t="s">
         <v>135</v>
       </c>
       <c r="C189" t="s">
-        <v>265</v>
+        <v>157</v>
       </c>
       <c r="E189" t="s">
         <v>200</v>
@@ -4151,13 +4190,13 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="B190" t="s">
         <v>135</v>
       </c>
       <c r="C190" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="E190" t="s">
         <v>200</v>
@@ -4165,13 +4204,13 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>160</v>
+        <v>263</v>
       </c>
       <c r="B191" t="s">
         <v>135</v>
       </c>
       <c r="C191" t="s">
-        <v>160</v>
+        <v>263</v>
       </c>
       <c r="E191" t="s">
         <v>200</v>
@@ -4179,13 +4218,13 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>266</v>
+        <v>304</v>
       </c>
       <c r="B192" t="s">
         <v>135</v>
       </c>
       <c r="C192" t="s">
-        <v>266</v>
+        <v>304</v>
       </c>
       <c r="E192" t="s">
         <v>200</v>
@@ -4193,13 +4232,13 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B193" t="s">
         <v>135</v>
       </c>
       <c r="C193" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E193" t="s">
         <v>200</v>
@@ -4207,13 +4246,13 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>162</v>
+        <v>264</v>
       </c>
       <c r="B194" t="s">
         <v>135</v>
       </c>
       <c r="C194" t="s">
-        <v>162</v>
+        <v>264</v>
       </c>
       <c r="E194" t="s">
         <v>200</v>
@@ -4221,13 +4260,13 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>163</v>
+        <v>265</v>
       </c>
       <c r="B195" t="s">
         <v>135</v>
       </c>
       <c r="C195" t="s">
-        <v>163</v>
+        <v>265</v>
       </c>
       <c r="E195" t="s">
         <v>200</v>
@@ -4235,13 +4274,13 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>267</v>
+        <v>159</v>
       </c>
       <c r="B196" t="s">
         <v>135</v>
       </c>
       <c r="C196" t="s">
-        <v>268</v>
+        <v>159</v>
       </c>
       <c r="E196" t="s">
         <v>200</v>
@@ -4249,13 +4288,13 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>164</v>
+        <v>317</v>
       </c>
       <c r="B197" t="s">
         <v>135</v>
       </c>
       <c r="C197" t="s">
-        <v>164</v>
+        <v>317</v>
       </c>
       <c r="E197" t="s">
         <v>200</v>
@@ -4263,13 +4302,13 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>269</v>
+        <v>160</v>
       </c>
       <c r="B198" t="s">
         <v>135</v>
       </c>
       <c r="C198" t="s">
-        <v>269</v>
+        <v>160</v>
       </c>
       <c r="E198" t="s">
         <v>200</v>
@@ -4277,13 +4316,13 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>165</v>
+        <v>266</v>
       </c>
       <c r="B199" t="s">
         <v>135</v>
       </c>
       <c r="C199" t="s">
-        <v>165</v>
+        <v>266</v>
       </c>
       <c r="E199" t="s">
         <v>200</v>
@@ -4291,13 +4330,13 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B200" t="s">
         <v>135</v>
       </c>
       <c r="C200" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E200" t="s">
         <v>200</v>
@@ -4305,13 +4344,13 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B201" t="s">
         <v>135</v>
       </c>
       <c r="C201" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E201" t="s">
         <v>200</v>
@@ -4319,13 +4358,13 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B202" t="s">
         <v>135</v>
       </c>
       <c r="C202" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E202" t="s">
         <v>200</v>
@@ -4333,13 +4372,13 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B203" t="s">
         <v>135</v>
       </c>
       <c r="C203" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E203" t="s">
         <v>200</v>
@@ -4347,13 +4386,13 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B204" t="s">
         <v>135</v>
       </c>
       <c r="C204" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E204" t="s">
         <v>200</v>
@@ -4361,13 +4400,13 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>170</v>
+        <v>269</v>
       </c>
       <c r="B205" t="s">
         <v>135</v>
       </c>
       <c r="C205" t="s">
-        <v>170</v>
+        <v>269</v>
       </c>
       <c r="E205" t="s">
         <v>200</v>
@@ -4375,13 +4414,13 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>271</v>
+        <v>165</v>
       </c>
       <c r="B206" t="s">
         <v>135</v>
       </c>
       <c r="C206" t="s">
-        <v>271</v>
+        <v>165</v>
       </c>
       <c r="E206" t="s">
         <v>200</v>
@@ -4389,13 +4428,13 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>272</v>
+        <v>166</v>
       </c>
       <c r="B207" t="s">
         <v>135</v>
       </c>
       <c r="C207" t="s">
-        <v>273</v>
+        <v>166</v>
       </c>
       <c r="E207" t="s">
         <v>200</v>
@@ -4403,258 +4442,237 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>167</v>
+      </c>
+      <c r="B208" t="s">
+        <v>135</v>
+      </c>
+      <c r="C208" t="s">
+        <v>167</v>
+      </c>
+      <c r="E208" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>168</v>
+      </c>
+      <c r="B209" t="s">
+        <v>135</v>
+      </c>
+      <c r="C209" t="s">
+        <v>168</v>
+      </c>
+      <c r="E209" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>270</v>
+      </c>
+      <c r="B210" t="s">
+        <v>135</v>
+      </c>
+      <c r="C210" t="s">
+        <v>270</v>
+      </c>
+      <c r="E210" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>169</v>
+      </c>
+      <c r="B211" t="s">
+        <v>135</v>
+      </c>
+      <c r="C211" t="s">
+        <v>169</v>
+      </c>
+      <c r="E211" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>170</v>
+      </c>
+      <c r="B212" t="s">
+        <v>135</v>
+      </c>
+      <c r="C212" t="s">
+        <v>170</v>
+      </c>
+      <c r="E212" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>271</v>
+      </c>
+      <c r="B213" t="s">
+        <v>135</v>
+      </c>
+      <c r="C213" t="s">
+        <v>271</v>
+      </c>
+      <c r="E213" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>272</v>
+      </c>
+      <c r="B214" t="s">
+        <v>135</v>
+      </c>
+      <c r="C214" t="s">
+        <v>273</v>
+      </c>
+      <c r="E214" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>274</v>
       </c>
-      <c r="B208" t="s">
-        <v>135</v>
-      </c>
-      <c r="C208" t="s">
+      <c r="B215" t="s">
+        <v>135</v>
+      </c>
+      <c r="C215" t="s">
         <v>274</v>
       </c>
-      <c r="E208" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+      <c r="E215" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>171</v>
       </c>
-      <c r="B209" t="s">
-        <v>135</v>
-      </c>
-      <c r="C209" t="s">
+      <c r="B216" t="s">
+        <v>135</v>
+      </c>
+      <c r="C216" t="s">
         <v>171</v>
       </c>
-      <c r="E209" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+      <c r="E216" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>275</v>
       </c>
-      <c r="B210" t="s">
-        <v>135</v>
-      </c>
-      <c r="C210" t="s">
+      <c r="B217" t="s">
+        <v>135</v>
+      </c>
+      <c r="C217" t="s">
         <v>275</v>
       </c>
-      <c r="E210" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+      <c r="E217" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>276</v>
       </c>
-      <c r="B211" t="s">
-        <v>135</v>
-      </c>
-      <c r="C211" t="s">
+      <c r="B218" t="s">
+        <v>135</v>
+      </c>
+      <c r="C218" t="s">
         <v>276</v>
       </c>
-      <c r="E211" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+      <c r="E218" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>172</v>
       </c>
-      <c r="B212" t="s">
-        <v>135</v>
-      </c>
-      <c r="C212" t="s">
+      <c r="B219" t="s">
+        <v>135</v>
+      </c>
+      <c r="C219" t="s">
         <v>172</v>
       </c>
-      <c r="E212" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+      <c r="E219" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
         <v>277</v>
       </c>
-      <c r="B213" t="s">
-        <v>135</v>
-      </c>
-      <c r="C213" t="s">
+      <c r="B220" t="s">
+        <v>135</v>
+      </c>
+      <c r="C220" t="s">
         <v>277</v>
       </c>
-      <c r="E213" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+      <c r="E220" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>278</v>
       </c>
-      <c r="B214" t="s">
-        <v>135</v>
-      </c>
-      <c r="C214" t="s">
+      <c r="B221" t="s">
+        <v>135</v>
+      </c>
+      <c r="C221" t="s">
         <v>278</v>
       </c>
-      <c r="E214" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+      <c r="E221" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>279</v>
       </c>
-      <c r="B215" t="s">
-        <v>135</v>
-      </c>
-      <c r="C215" t="s">
+      <c r="B222" t="s">
+        <v>135</v>
+      </c>
+      <c r="C222" t="s">
         <v>279</v>
       </c>
-      <c r="E215" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+      <c r="E222" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>280</v>
       </c>
-      <c r="B216" t="s">
-        <v>135</v>
-      </c>
-      <c r="C216" t="s">
+      <c r="B223" t="s">
+        <v>135</v>
+      </c>
+      <c r="C223" t="s">
         <v>280</v>
       </c>
-      <c r="E216" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+      <c r="E223" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>281</v>
       </c>
-      <c r="B217" t="s">
-        <v>135</v>
-      </c>
-      <c r="C217" t="s">
+      <c r="B224" t="s">
+        <v>135</v>
+      </c>
+      <c r="C224" t="s">
         <v>281</v>
-      </c>
-      <c r="E217" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>305</v>
-      </c>
-      <c r="B218" t="s">
-        <v>135</v>
-      </c>
-      <c r="C218" t="s">
-        <v>305</v>
-      </c>
-      <c r="E218" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>282</v>
-      </c>
-      <c r="B219" t="s">
-        <v>135</v>
-      </c>
-      <c r="C219" t="s">
-        <v>283</v>
-      </c>
-      <c r="E219" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>173</v>
-      </c>
-      <c r="B220" t="s">
-        <v>135</v>
-      </c>
-      <c r="C220" t="s">
-        <v>173</v>
-      </c>
-      <c r="D220" t="s">
-        <v>219</v>
-      </c>
-      <c r="E220" t="s">
-        <v>200</v>
-      </c>
-      <c r="F220">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>174</v>
-      </c>
-      <c r="B221" t="s">
-        <v>135</v>
-      </c>
-      <c r="C221" t="s">
-        <v>11</v>
-      </c>
-      <c r="E221" t="s">
-        <v>200</v>
-      </c>
-      <c r="F221">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>11</v>
-      </c>
-      <c r="B222" t="s">
-        <v>135</v>
-      </c>
-      <c r="C222" t="s">
-        <v>11</v>
-      </c>
-      <c r="D222" t="s">
-        <v>220</v>
-      </c>
-      <c r="E222" t="s">
-        <v>200</v>
-      </c>
-      <c r="F222">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>3</v>
-      </c>
-      <c r="B223" t="s">
-        <v>135</v>
-      </c>
-      <c r="C223" t="s">
-        <v>11</v>
-      </c>
-      <c r="D223" t="s">
-        <v>220</v>
-      </c>
-      <c r="E223" t="s">
-        <v>200</v>
-      </c>
-      <c r="F223">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>175</v>
-      </c>
-      <c r="B224" t="s">
-        <v>135</v>
-      </c>
-      <c r="C224" t="s">
-        <v>175</v>
       </c>
       <c r="E224" t="s">
         <v>200</v>
@@ -4662,13 +4680,13 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>176</v>
+        <v>305</v>
       </c>
       <c r="B225" t="s">
         <v>135</v>
       </c>
       <c r="C225" t="s">
-        <v>176</v>
+        <v>305</v>
       </c>
       <c r="E225" t="s">
         <v>200</v>
@@ -4676,13 +4694,13 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>177</v>
+        <v>282</v>
       </c>
       <c r="B226" t="s">
         <v>135</v>
       </c>
       <c r="C226" t="s">
-        <v>177</v>
+        <v>283</v>
       </c>
       <c r="E226" t="s">
         <v>200</v>
@@ -4690,13 +4708,13 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>178</v>
+        <v>319</v>
       </c>
       <c r="B227" t="s">
         <v>135</v>
       </c>
       <c r="C227" t="s">
-        <v>178</v>
+        <v>319</v>
       </c>
       <c r="E227" t="s">
         <v>200</v>
@@ -4704,69 +4722,90 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B228" t="s">
         <v>135</v>
       </c>
       <c r="C228" t="s">
-        <v>179</v>
+        <v>173</v>
+      </c>
+      <c r="D228" t="s">
+        <v>219</v>
       </c>
       <c r="E228" t="s">
         <v>200</v>
+      </c>
+      <c r="F228">
+        <v>3</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B229" t="s">
         <v>135</v>
       </c>
       <c r="C229" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
       <c r="E229" t="s">
         <v>200</v>
+      </c>
+      <c r="F229">
+        <v>1</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>181</v>
+        <v>11</v>
       </c>
       <c r="B230" t="s">
         <v>135</v>
       </c>
       <c r="C230" t="s">
-        <v>181</v>
+        <v>11</v>
+      </c>
+      <c r="D230" t="s">
+        <v>220</v>
       </c>
       <c r="E230" t="s">
         <v>200</v>
+      </c>
+      <c r="F230">
+        <v>1</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>182</v>
+        <v>3</v>
       </c>
       <c r="B231" t="s">
         <v>135</v>
       </c>
       <c r="C231" t="s">
-        <v>182</v>
+        <v>11</v>
+      </c>
+      <c r="D231" t="s">
+        <v>220</v>
       </c>
       <c r="E231" t="s">
         <v>200</v>
+      </c>
+      <c r="F231">
+        <v>1</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B232" t="s">
         <v>135</v>
       </c>
       <c r="C232" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E232" t="s">
         <v>200</v>
@@ -4774,93 +4813,69 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B233" t="s">
         <v>135</v>
       </c>
       <c r="C233" t="s">
-        <v>185</v>
-      </c>
-      <c r="D233" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="E233" t="s">
-        <v>201</v>
-      </c>
-      <c r="F233">
-        <v>2</v>
+        <v>200</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B234" t="s">
         <v>135</v>
       </c>
       <c r="C234" t="s">
-        <v>185</v>
-      </c>
-      <c r="D234" t="s">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="E234" t="s">
-        <v>201</v>
-      </c>
-      <c r="F234">
-        <v>2</v>
+        <v>200</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B235" t="s">
         <v>135</v>
       </c>
       <c r="C235" t="s">
-        <v>185</v>
-      </c>
-      <c r="D235" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
       <c r="E235" t="s">
-        <v>201</v>
-      </c>
-      <c r="F235">
-        <v>2</v>
+        <v>200</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B236" t="s">
         <v>135</v>
       </c>
       <c r="C236" t="s">
-        <v>185</v>
-      </c>
-      <c r="D236" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="E236" t="s">
-        <v>201</v>
-      </c>
-      <c r="F236">
-        <v>2</v>
+        <v>200</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>284</v>
+        <v>180</v>
       </c>
       <c r="B237" t="s">
         <v>135</v>
       </c>
       <c r="C237" t="s">
-        <v>284</v>
+        <v>180</v>
       </c>
       <c r="E237" t="s">
         <v>200</v>
@@ -4868,13 +4883,13 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>306</v>
+        <v>181</v>
       </c>
       <c r="B238" t="s">
         <v>135</v>
       </c>
       <c r="C238" t="s">
-        <v>306</v>
+        <v>181</v>
       </c>
       <c r="E238" t="s">
         <v>200</v>
@@ -4882,13 +4897,13 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>285</v>
+        <v>182</v>
       </c>
       <c r="B239" t="s">
         <v>135</v>
       </c>
       <c r="C239" t="s">
-        <v>285</v>
+        <v>182</v>
       </c>
       <c r="E239" t="s">
         <v>200</v>
@@ -4896,13 +4911,13 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B240" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C240" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E240" t="s">
         <v>200</v>
@@ -4910,47 +4925,59 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>307</v>
+        <v>184</v>
       </c>
       <c r="B241" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C241" t="s">
-        <v>307</v>
+        <v>185</v>
+      </c>
+      <c r="D241" t="s">
+        <v>215</v>
       </c>
       <c r="E241" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="F241">
+        <v>2</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>286</v>
+        <v>186</v>
       </c>
       <c r="B242" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C242" t="s">
-        <v>286</v>
+        <v>185</v>
+      </c>
+      <c r="D242" t="s">
+        <v>215</v>
       </c>
       <c r="E242" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="F242">
+        <v>2</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>0</v>
+        <v>187</v>
       </c>
       <c r="B243" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C243" t="s">
-        <v>1</v>
+        <v>185</v>
       </c>
       <c r="D243" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E243" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F243">
         <v>2</v>
@@ -4958,33 +4985,33 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="B244" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C244" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="D244" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E244" t="s">
         <v>201</v>
       </c>
       <c r="F244">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>191</v>
+        <v>284</v>
       </c>
       <c r="B245" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C245" t="s">
-        <v>191</v>
+        <v>284</v>
       </c>
       <c r="E245" t="s">
         <v>200</v>
@@ -4992,13 +5019,13 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>192</v>
+        <v>306</v>
       </c>
       <c r="B246" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C246" t="s">
-        <v>192</v>
+        <v>306</v>
       </c>
       <c r="E246" t="s">
         <v>200</v>
@@ -5006,13 +5033,13 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>193</v>
+        <v>285</v>
       </c>
       <c r="B247" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C247" t="s">
-        <v>193</v>
+        <v>285</v>
       </c>
       <c r="E247" t="s">
         <v>200</v>
@@ -5020,13 +5047,13 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B248" t="s">
         <v>189</v>
       </c>
       <c r="C248" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E248" t="s">
         <v>200</v>
@@ -5034,13 +5061,13 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>196</v>
+        <v>307</v>
       </c>
       <c r="B249" t="s">
         <v>189</v>
       </c>
       <c r="C249" t="s">
-        <v>196</v>
+        <v>307</v>
       </c>
       <c r="E249" t="s">
         <v>200</v>
@@ -5048,13 +5075,13 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>197</v>
+        <v>314</v>
       </c>
       <c r="B250" t="s">
         <v>189</v>
       </c>
       <c r="C250" t="s">
-        <v>197</v>
+        <v>314</v>
       </c>
       <c r="E250" t="s">
         <v>200</v>
@@ -5062,20 +5089,158 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
       <c r="B251" t="s">
         <v>189</v>
       </c>
       <c r="C251" t="s">
+        <v>286</v>
+      </c>
+      <c r="E251" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>0</v>
+      </c>
+      <c r="B252" t="s">
+        <v>189</v>
+      </c>
+      <c r="C252" t="s">
+        <v>1</v>
+      </c>
+      <c r="D252" t="s">
+        <v>221</v>
+      </c>
+      <c r="E252" t="s">
+        <v>200</v>
+      </c>
+      <c r="F252">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>2</v>
+      </c>
+      <c r="B253" t="s">
+        <v>189</v>
+      </c>
+      <c r="C253" t="s">
+        <v>203</v>
+      </c>
+      <c r="D253" t="s">
+        <v>213</v>
+      </c>
+      <c r="E253" t="s">
+        <v>201</v>
+      </c>
+      <c r="F253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>191</v>
+      </c>
+      <c r="B254" t="s">
+        <v>189</v>
+      </c>
+      <c r="C254" t="s">
+        <v>191</v>
+      </c>
+      <c r="E254" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>192</v>
+      </c>
+      <c r="B255" t="s">
+        <v>189</v>
+      </c>
+      <c r="C255" t="s">
+        <v>192</v>
+      </c>
+      <c r="E255" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>193</v>
+      </c>
+      <c r="B256" t="s">
+        <v>189</v>
+      </c>
+      <c r="C256" t="s">
+        <v>193</v>
+      </c>
+      <c r="E256" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>194</v>
+      </c>
+      <c r="B257" t="s">
+        <v>189</v>
+      </c>
+      <c r="C257" t="s">
+        <v>195</v>
+      </c>
+      <c r="E257" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>196</v>
+      </c>
+      <c r="B258" t="s">
+        <v>189</v>
+      </c>
+      <c r="C258" t="s">
+        <v>196</v>
+      </c>
+      <c r="E258" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>197</v>
+      </c>
+      <c r="B259" t="s">
+        <v>189</v>
+      </c>
+      <c r="C259" t="s">
+        <v>197</v>
+      </c>
+      <c r="E259" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
         <v>308</v>
       </c>
-      <c r="E251" t="s">
+      <c r="B260" t="s">
+        <v>189</v>
+      </c>
+      <c r="C260" t="s">
+        <v>308</v>
+      </c>
+      <c r="E260" t="s">
         <v>200</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E173">
+  <sortState ref="A2:E178">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>